<commit_message>
Added Final BOM Table
</commit_message>
<xml_diff>
--- a/RocketHat.xlsx
+++ b/RocketHat.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armstrjj\Documents\Custom Electronics\RocketHat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4F6EE6F7-4326-4C96-8C56-111ABE6DFB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBD7F1-AE28-4789-A693-EF20B2809B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RocketHat" sheetId="1" r:id="rId1"/>
+    <sheet name="Final BOM" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
   <si>
     <t>Source:</t>
   </si>
@@ -272,12 +285,60 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Quanitity</t>
+  </si>
+  <si>
+    <t>Purchase Link</t>
+  </si>
+  <si>
+    <t>1608 Metric Resistor Book</t>
+  </si>
+  <si>
+    <t>RQ5C035BCTCL - P Channel Mosfet</t>
+  </si>
+  <si>
+    <t>Price Per Unit</t>
+  </si>
+  <si>
+    <t>2N3904 NTE Electronics, Inc | Discrete Semiconductor Products | DigiKey Marketplace</t>
+  </si>
+  <si>
+    <t>NPN Transistor 40</t>
+  </si>
+  <si>
+    <t>2-Wire Terminal Block 16-26 AWG</t>
+  </si>
+  <si>
+    <t>Xbee Header Block Bag of 10</t>
+  </si>
+  <si>
+    <t>Generic 2mm 10 Pin XBee Socket Header(pack of 10) - - Amazon.com</t>
+  </si>
+  <si>
+    <t>Itemized Cost</t>
+  </si>
+  <si>
+    <t>Total Order Cost</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Header Socket</t>
+  </si>
+  <si>
+    <t>Amazon.com: Adafruit 4079 2 x 20 Socket Riser Header for Raspberry Pi Hats and Bonnets : Electronics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +780,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -763,13 +824,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -797,6 +861,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="43" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1123,11 +1188,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,12 +1660,178 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1" display="https://www.digikey.com/en/products/detail/on-shore-technology-inc/OSTTE020104/2351816"/>
-    <hyperlink ref="G25" r:id="rId2" display="https://www.digikey.com/en/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262"/>
-    <hyperlink ref="G33" r:id="rId3" display="https://www.digikey.com/en/products/detail/galco-industrial-electronics/2N3904/15657702"/>
-    <hyperlink ref="G35" r:id="rId4" display="https://www.digikey.com/en/products/detail/rohm-semiconductor/RQ5C035BCTCL/6573257"/>
-    <hyperlink ref="G43" r:id="rId5" display="https://www.digikey.com/en/products/detail/stackpole-electronics-inc/KIT-RMCF0603JT-13/4916518"/>
+    <hyperlink ref="G23" r:id="rId1" display="https://www.digikey.com/en/products/detail/on-shore-technology-inc/OSTTE020104/2351816" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G25" r:id="rId2" display="https://www.digikey.com/en/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G33" r:id="rId3" display="https://www.digikey.com/en/products/detail/galco-industrial-electronics/2N3904/15657702" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G35" r:id="rId4" display="https://www.digikey.com/en/products/detail/rohm-semiconductor/RQ5C035BCTCL/6573257" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G43" r:id="rId5" display="https://www.digikey.com/en/products/detail/stackpole-electronics-inc/KIT-RMCF0603JT-13/4916518" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B82CE3-AD6B-4338-BFFA-26415943B100}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="68.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="3">
+        <v>26.96</v>
+      </c>
+      <c r="E2" s="3">
+        <f>B2*D2</f>
+        <v>26.96</v>
+      </c>
+      <c r="F2" s="4">
+        <f>SUM(E:E)</f>
+        <v>50.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E9" si="0">B3*D3</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.99</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://www.digikey.com/en/products/detail/stackpole-electronics-inc/KIT-RMCF0603JT-13/4916518" xr:uid="{50F6195C-E9E5-4790-99A7-4CCD72CBFADE}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.digikey.com/en/products/detail/rohm-semiconductor/RQ5C035BCTCL/6573257" xr:uid="{E8A91053-1CF7-4A9B-89F0-059D782F16BE}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/2N3904/11648305" xr:uid="{FCB2C559-A9A9-4115-9E98-0612514F4781}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://www.digikey.com/en/products/detail/on-shore-technology-inc/OSTTE020104/2351816" xr:uid="{B7DC30C1-2046-47F1-BB8A-CD3E82C1F397}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://www.amazon.com/Generic-XBee-Socket-Header-pack/dp/B00OE92P88/ref=sr_1_1?crid=1UO6O2H5M0R1U&amp;keywords=XBee+socket+header&amp;qid=1645056431&amp;sprefix=xbee+socket+heade%2Caps%2C62&amp;sr=8-1" xr:uid="{C967F94A-1F95-40E6-9D58-51C83C503E67}"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://www.amazon.com/Adafruit-Socket-Header-Raspberry-Bonnets/dp/B07PPD25MK/ref=sr_1_7?crid=3SJNFW4ITDQDK&amp;keywords=Raspberry+PI+gpio+socket&amp;qid=1645056292&amp;sprefix=raspberry+pi+gpio+socket%2Caps%2C77&amp;sr=8-7" xr:uid="{607DF7D3-9933-4EEA-961E-83E39125E9D9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>